<commit_message>
v3.3 veri girişleri güncel
</commit_message>
<xml_diff>
--- a/data/belgrad/BEL25_FRACAS.xlsx
+++ b/data/belgrad/BEL25_FRACAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="BuÇalışmaKitabı"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FRACAS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FRACAS" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
+    <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+    <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="Ana_Kompanent">#REF!</definedName>
@@ -855,8 +855,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Anasayfa"/>
       <sheetName val="1. Araç Kalite Kontrol Verileri"/>
@@ -894,8 +894,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover"/>
       <sheetName val="Overview"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="AA1" s="14" t="inlineStr">
         <is>
-          <t>Adeti</t>
+          <t>Adet</t>
         </is>
       </c>
       <c r="AB1" s="16" t="inlineStr">

</xml_diff>